<commit_message>
Added download function and success message
</commit_message>
<xml_diff>
--- a/admin@admin.ruJobEvaluation.xlsx
+++ b/admin@admin.ruJobEvaluation.xlsx
@@ -472,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="W5" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Y5" s="4" t="inlineStr">
@@ -628,175 +628,175 @@
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Jopa1</t>
+          <t>Natasha</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>I</t>
         </is>
       </c>
       <c r="I6" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K6" s="4" t="n">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="M6" s="4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O6" s="4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="S6" s="4" t="n">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="U6" s="4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="W6" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Y6" s="4" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AA6" s="4" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Jopa2</t>
+          <t>Popka</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I7" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>230</v>
+      </c>
+      <c r="M7" s="4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="O7" s="4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q7" s="4" t="n">
+        <v>43</v>
+      </c>
+      <c r="S7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="U7" s="4" t="inlineStr">
+        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>II</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>152</v>
-      </c>
-      <c r="M7" s="4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
+      <c r="W7" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="Q7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4" t="n">
-        <v>38</v>
-      </c>
-      <c r="U7" s="4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="W7" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="Y7" s="4" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AA7" s="4" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Jopa</t>
+          <t>Sisechki</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>III</t>
         </is>
       </c>
       <c r="I8" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K8" s="4" t="n">
-        <v>152</v>
+        <v>528</v>
       </c>
       <c r="M8" s="4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="O8" s="4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Q8" s="4" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="S8" s="4" t="n">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="U8" s="4" t="inlineStr">
         <is>
@@ -805,37 +805,37 @@
       </c>
       <c r="W8" s="4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>I</t>
         </is>
       </c>
       <c r="AA8" s="4" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Jopa124</t>
+          <t>Ssadasd</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>H</t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>IV</t>
         </is>
       </c>
       <c r="I9" s="4" t="inlineStr">
@@ -844,11 +844,11 @@
         </is>
       </c>
       <c r="K9" s="4" t="n">
-        <v>700</v>
+        <v>1216</v>
       </c>
       <c r="M9" s="4" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>H</t>
         </is>
       </c>
       <c r="O9" s="4" t="inlineStr">
@@ -857,96 +857,224 @@
         </is>
       </c>
       <c r="Q9" s="4" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="S9" s="4" t="n">
-        <v>400</v>
+        <v>1056</v>
       </c>
       <c r="U9" s="4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>H</t>
         </is>
       </c>
       <c r="W9" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>S</t>
         </is>
       </c>
       <c r="AA9" s="4" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>Piska</t>
+          <t>Safsdf</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I10" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K10" s="4" t="n">
+        <v>230</v>
+      </c>
+      <c r="M10" s="4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="O10" s="4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Q10" s="4" t="n">
+        <v>43</v>
+      </c>
+      <c r="S10" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="U10" s="4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="W10" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Y10" s="4" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="AA10" s="4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Zhopa</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
           <t>D</t>
         </is>
       </c>
-      <c r="G10" s="4" t="inlineStr">
-        <is>
-          <t>II</t>
-        </is>
-      </c>
-      <c r="I10" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K10" s="4" t="n">
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="I11" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K11" s="4" t="n">
         <v>175</v>
       </c>
-      <c r="M10" s="4" t="inlineStr">
+      <c r="M11" s="4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="O11" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q11" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="S11" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="U11" s="4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W11" s="4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Y11" s="4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AA11" s="4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Pisya</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="O10" s="4" t="inlineStr">
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>III</t>
+        </is>
+      </c>
+      <c r="I12" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="M12" s="4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="O12" s="4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="Q10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="4" t="n">
+      <c r="Q12" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="S12" s="4" t="n">
         <v>57</v>
       </c>
-      <c r="U10" s="4" t="inlineStr">
+      <c r="U12" s="4" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="W10" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y10" s="4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AA10" s="4" t="n">
+      <c r="W12" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Y12" s="4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AA12" s="4" t="n">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="93">
+  <mergeCells count="119">
     <mergeCell ref="B1:Z2"/>
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="C3:D4"/>
@@ -1040,6 +1168,32 @@
     <mergeCell ref="U10:V10"/>
     <mergeCell ref="W10:X10"/>
     <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="Y12:Z12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>